<commit_message>
feat: finish tests models
</commit_message>
<xml_diff>
--- a/outputs/mamografia/Testes Modelos.xlsx
+++ b/outputs/mamografia/Testes Modelos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\Radiomica\outputs\mamografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE29D1F-E1AD-444F-9BDD-E35BE0C7AAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF0066-4EE2-4FFC-9F5B-1A7BCA0E534C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{9A836E04-45DA-4314-8960-634297EE0671}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{9A836E04-45DA-4314-8960-634297EE0671}"/>
   </bookViews>
   <sheets>
     <sheet name="Mias" sheetId="1" r:id="rId1"/>
-    <sheet name="INBreast" sheetId="2" r:id="rId2"/>
-    <sheet name="CMMD" sheetId="3" r:id="rId3"/>
+    <sheet name="CBIS-DDSM" sheetId="4" r:id="rId2"/>
+    <sheet name="INBreast" sheetId="2" r:id="rId3"/>
+    <sheet name="CMMD" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="23">
   <si>
     <t>Imagem</t>
   </si>
@@ -249,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,16 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,9 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -321,6 +310,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -337,24 +344,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -680,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DB01F-8831-4E65-A143-895D46C42CCD}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,1179 +716,1179 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="21">
+      <c r="C2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="17">
         <v>0.57142857000000002</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="11">
         <v>0.58333332999999998</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="11">
         <v>0.52380952000000003</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="11">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>0.55952380999999995</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="21">
+      <c r="G4" s="22"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>0.57142857000000002</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="37" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="21">
+      <c r="I5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="A6" s="22"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17">
         <v>0.58333334000000003</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="12">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>0.53571429000000004</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="12">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="38" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="C8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="17">
         <v>0.61904762000000002</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="38" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="21">
+      <c r="I8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="17">
         <v>0.66666665999999997</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="A9" s="22"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="13">
         <v>0.55952380999999995</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="16">
+      <c r="G9" s="22"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="13">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="16">
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13">
         <v>0.61904762000000002</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="16">
+      <c r="G10" s="23"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="13">
         <v>0.53571429000000004</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="21">
+      <c r="C11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17">
         <v>0.57142857999999996</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="19">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="11">
         <v>0.5</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="21">
+      <c r="G12" s="22"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="17">
         <v>0.61904762000000002</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>0.39285713999999999</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="36"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="26"/>
       <c r="I13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="11">
         <v>0.53571429000000004</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="21">
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="17">
         <v>0.5</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="25" t="s">
+      <c r="G14" s="22"/>
+      <c r="H14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="12">
         <v>0.58333332999999998</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>0.47619046999999998</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="21">
+      <c r="G15" s="22"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="17">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>0.5</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="29"/>
       <c r="I16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="12">
         <v>0.55952380999999995</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="C17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="13">
         <v>0.57142857999999996</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="28" t="s">
+      <c r="G17" s="22"/>
+      <c r="H17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="16">
+      <c r="I17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="13">
         <v>0.58333332999999998</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="21">
+      <c r="A18" s="22"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="17">
         <v>0.58333332999999998</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="21">
+      <c r="G18" s="22"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="A19" s="23"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13">
         <v>0.57142857000000002</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="16">
+      <c r="G19" s="23"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="13">
         <v>0.55952380999999995</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="21">
+      <c r="C20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17">
         <v>0.52380952000000003</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="11">
         <v>0.55952380999999995</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <v>0.42857142999999998</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="21">
+      <c r="G21" s="22"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="11">
         <v>0.46428571000000002</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="36"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="26"/>
       <c r="I22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="11">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="25" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>0.64285714000000005</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="25" t="s">
+      <c r="G23" s="22"/>
+      <c r="H23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="21">
+      <c r="I23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="17">
         <v>0.65476190000000001</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="21">
+      <c r="A24" s="22"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="17">
         <v>0.67857142999999998</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="26"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="12">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="12">
         <v>0.5</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="27"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="12">
         <v>0.63095237999999998</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="28" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="16">
+      <c r="C26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="13">
         <v>0.59523809000000005</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="28" t="s">
+      <c r="G26" s="22"/>
+      <c r="H26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="16">
+      <c r="I26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="13">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="21">
+      <c r="A27" s="22"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="17">
         <v>0.60714285999999995</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="21">
+      <c r="G27" s="22"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="16">
+      <c r="A28" s="23"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="13">
         <v>0.60714285999999995</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="16">
+      <c r="G28" s="23"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="13">
         <v>0.63095237999999998</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="11">
         <v>0.47619048000000003</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="H29" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="11">
         <v>0.52380952000000003</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="21">
+      <c r="A30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="17">
         <v>0.53571427999999999</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="35"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="11">
         <v>0.53571429000000004</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="36"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="11">
         <v>0.39285713999999999</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="21">
+      <c r="G31" s="22"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="17">
         <v>0.55952380999999995</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="25" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="21">
+      <c r="C32" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="17">
         <v>0.61904762000000002</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="25" t="s">
+      <c r="G32" s="22"/>
+      <c r="H32" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="12">
         <v>0.61904762000000002</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="14">
         <v>0.60714285999999995</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="26"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="12">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="12">
         <v>0.57142857000000002</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="21">
+      <c r="G34" s="22"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="17">
         <v>0.70238095</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="16">
+      <c r="C35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="13">
         <v>0.54761905</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="28" t="s">
+      <c r="G35" s="22"/>
+      <c r="H35" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I35" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="16">
+      <c r="I35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="13">
         <v>0.66666665999999997</v>
       </c>
-      <c r="L35" s="24"/>
+      <c r="L35" s="20"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="21">
+      <c r="A36" s="22"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="17">
         <v>0.64285714000000005</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="16">
+      <c r="G36" s="22"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="13">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="16">
+      <c r="A37" s="23"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="13">
         <v>0.53571429000000004</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J37" s="21">
+      <c r="G37" s="23"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="17">
         <v>0.69047619000000005</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="11">
         <v>0.42857142999999998</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="11">
         <v>0.52380952000000003</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="11">
         <v>0.53571429000000004</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="35"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="25"/>
       <c r="I39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="11">
         <v>0.59523809000000005</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="21">
+      <c r="A40" s="22"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="17">
         <v>0.57142857000000002</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" s="21">
+      <c r="G40" s="22"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="17">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="25" t="s">
+      <c r="A41" s="22"/>
+      <c r="B41" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="12">
         <v>0.42857142999999998</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="25" t="s">
+      <c r="G41" s="22"/>
+      <c r="H41" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I41" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="21">
+      <c r="I41" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="17">
         <v>0.63095237999999998</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="12">
         <v>0.53571429000000004</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="26"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="28"/>
       <c r="I42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="15">
+      <c r="J42" s="12">
         <v>0.63095237999999998</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="21">
+      <c r="A43" s="22"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="17">
         <v>0.60714285999999995</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="27"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="29"/>
       <c r="I43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="15">
+      <c r="J43" s="12">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="28" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="13">
         <v>0.5</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="28" t="s">
+      <c r="G44" s="22"/>
+      <c r="H44" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J44" s="16">
+      <c r="I44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="13">
         <v>0.60714285999999995</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="21">
+      <c r="A45" s="22"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="17">
         <v>0.60714285999999995</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" s="21">
+      <c r="G45" s="22"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="17">
         <v>0.67857142999999998</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="A46" s="23"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="13">
         <v>0.46428571000000002</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J46" s="16">
+      <c r="G46" s="23"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="13">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="21">
+      <c r="C47" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="17">
         <v>0.52380952999999997</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="34" t="s">
+      <c r="H47" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J47" s="14">
+      <c r="I47" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="17">
         <v>0.58333330000000005</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="11">
         <v>0.39285713</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="35"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="25"/>
       <c r="I48" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="11">
         <v>0.48809523999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="36"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="11">
         <v>0.42857142999999998</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="36"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="26"/>
       <c r="I49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="25" t="s">
+      <c r="A50" s="22"/>
+      <c r="B50" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="12">
         <v>0.54761905</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="25" t="s">
+      <c r="G50" s="22"/>
+      <c r="H50" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I50" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J50" s="15">
+      <c r="I50" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="17">
         <v>0.65476190000000001</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="21">
+      <c r="A51" s="22"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="17">
         <v>0.58333332999999998</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="26"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="28"/>
       <c r="I51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J51" s="15">
+      <c r="J51" s="12">
         <v>0.64285714000000005</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="12">
         <v>0.53571429000000004</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="27"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="29"/>
       <c r="I52" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J52" s="15">
+      <c r="J52" s="12">
         <v>0.57142857000000002</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="28" t="s">
+      <c r="A53" s="22"/>
+      <c r="B53" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="16">
+      <c r="C53" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="13">
         <v>0.52380952999999997</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="28" t="s">
+      <c r="G53" s="22"/>
+      <c r="H53" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="16">
+      <c r="I53" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="17">
         <v>0.61904762000000002</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="21">
+      <c r="A54" s="22"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="17">
         <v>0.58333332999999998</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J54" s="16">
+      <c r="G54" s="22"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="13">
         <v>0.58333332999999998</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="16">
+      <c r="A55" s="23"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="13">
         <v>0.57142857000000002</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J55" s="16">
+      <c r="G55" s="23"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" s="13">
         <v>0.53571429000000004</v>
       </c>
     </row>
@@ -2040,6 +2029,42 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="G38:G46"/>
+    <mergeCell ref="G47:G55"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="G20:G28"/>
+    <mergeCell ref="G29:G37"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="G11:G19"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A29:A37"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="A38:A46"/>
@@ -2052,42 +2077,6 @@
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="G2:G10"/>
-    <mergeCell ref="G11:G19"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="G20:G28"/>
-    <mergeCell ref="G29:G37"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="G38:G46"/>
-    <mergeCell ref="G47:G55"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="H47:H49"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2095,18 +2084,1210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4465909-35E8-45FE-931A-79F8B20087A0}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="I3:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.56228374000000003</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0.56401383999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.54152248999999997</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="17">
+        <v>0.58131487999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0.61072663999999999</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.56747404999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.61591695999999996</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.56401383999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.55190309999999998</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0.58304498000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.62629758000000002</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0.59688580999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.59861591999999997</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.57439446000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.5467128</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0.59169550000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.62456747000000001</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0.58304498000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.56228374000000003</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.51730103999999999</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.54844291000000001</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.57958478000000002</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.55190030999999995</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0.59861591999999997</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.57266435999999998</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.55536331999999999</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.56920415000000002</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0.52249135000000002</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0.55363322000000004</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0.50519002999999996</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.59515571</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.56574393999999995</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="17">
+        <v>0.61591695999999996</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.58477509000000005</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.56574393999999995</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="17">
+        <v>0.58823528999999997</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="17">
+        <v>0.58823528999999997</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.52249135000000002</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0.55017300999999996</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="17">
+        <v>0.58996539999999997</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="14">
+        <v>0.58131487999999998</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0.58996539999999997</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="13">
+        <v>0.58650519000000001</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="17">
+        <v>0.60553632999999996</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="13">
+        <v>0.58131487999999998</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0.5467128</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0.53114187000000002</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.52595155999999998</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.64013841000000005</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.56574393999999995</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0.60380623</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="13">
+        <v>0.58650519000000001</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="13">
+        <v>0.54844291000000001</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.58304498000000005</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="17">
+        <v>0.57439446000000005</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0.53806228</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.55017300999999996</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="B50" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="17">
+        <v>0.58304498000000005</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="12">
+        <v>0.53114187000000002</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" s="12"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="22"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0.56228374000000003</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52" s="12"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="22"/>
+      <c r="B53" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="17">
+        <v>0.57785467000000001</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="13"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="22"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0.54325259999999997</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="13"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0.56920415000000002</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="G47:G55"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="G38:G46"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="G29:G37"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="G20:G28"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G11:G19"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="H8:H10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651569A5-9BA8-437F-9622-9FA673467BEE}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
@@ -2142,246 +3323,408 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>0.57861635</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="11">
         <v>0.83962263999999998</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="13"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="13"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.63207546999999997</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.86477987000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0.65094339999999995</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0.86477912999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12">
         <v>0.69182390000000005</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="37" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="17">
         <v>0.89937107000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-    </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.66981131999999999</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.85220125999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.70440252000000003</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.88993710999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="13">
         <v>0.73270440000000003</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="38" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="16">
+      <c r="H8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="17">
         <v>0.90880503000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0.82704403000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.73899371000000003</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0.88993710000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="11">
         <v>0.58490565999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="25" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.63207546999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.62893082</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15">
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="17">
         <v>0.72012578999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="28" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.70754717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.69182390000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="C17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="13">
         <v>0.70440252000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="17">
+        <v>0.72641509000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.69811321000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B20" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="14">
+      <c r="C20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17">
         <v>0.59433961999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="25" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0.59119496999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0.57232704999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="15">
+      <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="12">
         <v>0.64150943000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="28" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="17">
+        <v>0.74213836</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="12">
+        <v>0.69811321000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="16">
+      <c r="C26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="13">
         <v>0.67610062999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="16"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.73899371000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="17">
+        <v>0.76100628999999997</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="F2:F10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52E74B4-4124-4438-BEA3-100B8C4EE76F}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,523 +3750,611 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="17">
         <v>0.67489712000000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="11">
+        <v>0.63844796999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="11">
+        <v>0.64197530999999997</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>0.66784244999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="15"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.67019399999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="12">
+        <v>0.66313933000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="38" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="C8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="17">
         <v>0.68018811999999995</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="16"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.66490300000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.67548501000000005</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="C11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17">
         <v>0.66490300000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="11">
+        <v>0.66666667000000002</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="11">
+        <v>0.59964726999999995</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="17">
         <v>0.67019399999999996</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="12">
+        <v>0.62433861999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="12">
+        <v>0.60846560999999999</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="C17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="17">
         <v>0.67724868000000005</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="16"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.64021163999999997</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="16"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.63315697000000004</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="14">
+      <c r="C20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17">
         <v>0.68724280000000004</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="11">
+        <v>0.64197530999999997</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="11">
+        <v>0.64550264999999996</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="25" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="15">
+      <c r="C23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="17">
         <v>0.69958847999999996</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="12">
+        <v>0.64021163999999997</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="12">
+        <v>0.67195766999999995</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="28" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="16">
+      <c r="C26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="17">
         <v>0.69782480999999996</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="16"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.64197530999999997</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="16"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.66490300000000002</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="11">
         <v>0.60728983000000003</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="14"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="17">
+        <v>0.69488536000000001</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="36"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="14"/>
+      <c r="D31" s="11">
+        <v>0.67195766999999995</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="25" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="12">
         <v>0.62669017999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="14">
+        <v>0.68253967999999998</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="15"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0.68253967999999998</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="16">
+      <c r="C35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="13">
         <v>0.62316285000000005</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="16"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.68606701999999997</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="16"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="17">
+        <v>0.69664903</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="14">
+      <c r="C38" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="17">
         <v>0.68959435999999996</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="11">
+        <v>0.57319224000000002</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="11">
+        <v>0.59788359999999996</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="25" t="s">
+      <c r="A41" s="22"/>
+      <c r="B41" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="15">
+      <c r="C41" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="17">
         <v>0.71075838000000002</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="15"/>
+      <c r="D42" s="12">
+        <v>0.59435625999999997</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="15"/>
+      <c r="D43" s="12">
+        <v>0.62786595999999995</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="28" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C44" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="17">
         <v>0.71781304999999995</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="16"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="13">
+        <v>0.57319224000000002</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="16"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.61728395000000003</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="11">
         <v>0.67901235000000004</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="14"/>
+      <c r="D48" s="11">
+        <v>0.67724868000000005</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="36"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="14"/>
+      <c r="D49" s="11">
+        <v>0.68430334999999998</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="25" t="s">
+      <c r="A50" s="22"/>
+      <c r="B50" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="12">
         <v>0.65255732</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="15"/>
+      <c r="D51" s="12">
+        <v>0.68430334999999998</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="15"/>
+      <c r="D52" s="12">
+        <v>0.67195766999999995</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="28" t="s">
+      <c r="A53" s="22"/>
+      <c r="B53" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="16">
+      <c r="C53" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="13">
         <v>0.65255732</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="16"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0.68783068999999997</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="16"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0.67724868000000005</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
@@ -2932,22 +4363,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: novos testes modelos
</commit_message>
<xml_diff>
--- a/outputs/mamografia/Testes Modelos.xlsx
+++ b/outputs/mamografia/Testes Modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\Radiomica\outputs\mamografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF0066-4EE2-4FFC-9F5B-1A7BCA0E534C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0464B962-B7F0-4DC6-A94A-85DD67B91AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{9A836E04-45DA-4314-8960-634297EE0671}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{9A836E04-45DA-4314-8960-634297EE0671}"/>
   </bookViews>
   <sheets>
     <sheet name="Mias" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="25">
   <si>
     <t>Imagem</t>
   </si>
@@ -107,6 +107,12 @@
   <si>
     <t>First Order + GLCM</t>
   </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>CLAHE ROI</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -310,6 +322,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -328,6 +346,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -344,12 +377,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92DB01F-8831-4E65-A143-895D46C42CCD}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +714,7 @@
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -700,1226 +727,277 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="24" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="17">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="24" t="s">
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.51849999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.58330000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.59250000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.47220000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.55549999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.52769999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.49980000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.49959999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.59250000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.46289999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.56469999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="11">
-        <v>0.58333332999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.52380952000000003</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="11">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0.55952380999999995</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="33" t="s">
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.54620000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.56469999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.62029999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="17">
-        <v>0.58333334000000003</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="12">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.53571429000000004</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="34" t="s">
+      <c r="C17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.4536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.62960000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.56469999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0.51849999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="22">
+        <v>0.59260000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="22">
+        <v>0.52769999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="17">
-        <v>0.61904762000000002</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="17">
-        <v>0.66666665999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.55952380999999995</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="13">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0.61904762000000002</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="13">
-        <v>0.53571429000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0.57142857999999996</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="17">
-        <v>0.61904762000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0.39285713999999999</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="11">
-        <v>0.53571429000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0.58333332999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0.47619046999999998</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="17">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="12">
-        <v>0.55952380999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="13">
-        <v>0.57142857999999996</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="13">
-        <v>0.58333332999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="17">
-        <v>0.58333332999999998</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="13">
-        <v>0.55952380999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="17">
-        <v>0.52380952000000003</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0.55952380999999995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.42857142999999998</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0.46428571000000002</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="11">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="12">
-        <v>0.64285714000000005</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="17">
-        <v>0.65476190000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="17">
-        <v>0.67857142999999998</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="C23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.56469999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.61102999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
       <c r="B25" s="29"/>
-      <c r="C25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="12">
-        <v>0.63095237999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0.59523809000000005</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="13">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="17">
-        <v>0.60714285999999995</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="13">
-        <v>0.60714285999999995</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="13">
-        <v>0.63095237999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="11">
-        <v>0.47619048000000003</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="11">
-        <v>0.52380952000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="17">
-        <v>0.53571427999999999</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="11">
-        <v>0.53571429000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0.39285713999999999</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="17">
-        <v>0.55952380999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="17">
-        <v>0.61904762000000002</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="12">
-        <v>0.61904762000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="14">
-        <v>0.60714285999999995</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="12">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="17">
-        <v>0.70238095</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="13">
-        <v>0.54761905</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="13">
-        <v>0.66666665999999997</v>
-      </c>
-      <c r="L35" s="20"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="13">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="13">
-        <v>0.53571429000000004</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J37" s="17">
-        <v>0.69047619000000005</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="11">
-        <v>0.42857142999999998</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="11">
-        <v>0.52380952000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="11">
-        <v>0.53571429000000004</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" s="11">
-        <v>0.59523809000000005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="17">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" s="17">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="12">
-        <v>0.42857142999999998</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="17">
-        <v>0.63095237999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="12">
-        <v>0.53571429000000004</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J42" s="12">
-        <v>0.63095237999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="17">
-        <v>0.60714285999999995</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J43" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J44" s="13">
-        <v>0.60714285999999995</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="17">
-        <v>0.60714285999999995</v>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" s="17">
-        <v>0.67857142999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="13">
-        <v>0.46428571000000002</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J46" s="13">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="17">
-        <v>0.52380952999999997</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J47" s="17">
-        <v>0.58333330000000005</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="11">
-        <v>0.39285713</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48" s="11">
-        <v>0.48809523999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="11">
-        <v>0.42857142999999998</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J49" s="11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="12">
-        <v>0.54761905</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I50" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J50" s="17">
-        <v>0.65476190000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="17">
-        <v>0.58333332999999998</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J51" s="12">
-        <v>0.64285714000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="12">
-        <v>0.53571429000000004</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J52" s="12">
-        <v>0.57142857000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="13">
-        <v>0.52380952999999997</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I53" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="17">
-        <v>0.61904762000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="17">
-        <v>0.58333332999999998</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J54" s="13">
-        <v>0.58333332999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="13">
-        <v>0.57142857000000002</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J55" s="13">
-        <v>0.53571429000000004</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0.61102999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="12:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="20"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1928,7 +1006,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1937,7 +1015,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1946,7 +1024,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1955,7 +1033,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1964,7 +1042,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2027,56 +1105,45 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="G38:G46"/>
-    <mergeCell ref="G47:G55"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="G20:G28"/>
-    <mergeCell ref="G29:G37"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="G2:G10"/>
-    <mergeCell ref="G11:G19"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H11:H13"/>
+  <mergeCells count="10">
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2087,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4465909-35E8-45FE-931A-79F8B20087A0}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J3" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
@@ -2134,10 +1201,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2148,10 +1215,10 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="7" t="s">
@@ -2162,8 +1229,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
@@ -2172,8 +1239,8 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="16" t="s">
         <v>21</v>
       </c>
@@ -2182,8 +1249,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
@@ -2192,8 +1259,8 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="7" t="s">
         <v>22</v>
       </c>
@@ -2202,8 +1269,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2214,8 +1281,8 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="33" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -2226,8 +1293,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
@@ -2236,8 +1303,8 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="9" t="s">
         <v>21</v>
       </c>
@@ -2246,8 +1313,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="18" t="s">
         <v>22</v>
       </c>
@@ -2256,8 +1323,8 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="18" t="s">
         <v>22</v>
       </c>
@@ -2266,8 +1333,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2278,8 +1345,8 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="34" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="10" t="s">
@@ -2290,8 +1357,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
@@ -2300,8 +1367,8 @@
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="34"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="16" t="s">
         <v>21</v>
       </c>
@@ -2310,8 +1377,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
@@ -2320,8 +1387,8 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="34"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="29"/>
       <c r="I10" s="10" t="s">
         <v>22</v>
       </c>
@@ -2330,10 +1397,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -2344,10 +1411,10 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="7" t="s">
@@ -2356,8 +1423,8 @@
       <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
@@ -2366,16 +1433,16 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="27"/>
       <c r="I12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
@@ -2384,16 +1451,16 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="28"/>
       <c r="I13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -2404,8 +1471,8 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="27" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -2414,8 +1481,8 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
@@ -2424,16 +1491,16 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="28"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="16" t="s">
         <v>22</v>
       </c>
@@ -2442,16 +1509,16 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="29"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -2462,8 +1529,8 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="30" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="37" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="10" t="s">
@@ -2472,8 +1539,8 @@
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
@@ -2482,16 +1549,16 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="31"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
@@ -2500,18 +1567,18 @@
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="32"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -2522,10 +1589,10 @@
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="7" t="s">
@@ -2534,8 +1601,8 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="16" t="s">
         <v>21</v>
       </c>
@@ -2544,16 +1611,16 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="25"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="27"/>
       <c r="I21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -2562,16 +1629,16 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="26"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="27" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2582,8 +1649,8 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="27" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I23" s="8" t="s">
@@ -2592,8 +1659,8 @@
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="8" t="s">
         <v>21</v>
       </c>
@@ -2602,16 +1669,16 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="28"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="16" t="s">
         <v>22</v>
       </c>
@@ -2620,16 +1687,16 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="29"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="12"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="30" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2640,8 +1707,8 @@
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="30" t="s">
+      <c r="G26" s="24"/>
+      <c r="H26" s="37" t="s">
         <v>6</v>
       </c>
       <c r="I26" s="10" t="s">
@@ -2650,8 +1717,8 @@
       <c r="J26" s="13"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="10" t="s">
         <v>21</v>
       </c>
@@ -2660,16 +1727,16 @@
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="31"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
@@ -2678,18 +1745,18 @@
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="32"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -2700,10 +1767,10 @@
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I29" s="7" t="s">
@@ -2712,8 +1779,8 @@
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="7" t="s">
         <v>21</v>
       </c>
@@ -2722,16 +1789,16 @@
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="25"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
@@ -2740,16 +1807,16 @@
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="26"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="27" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="16" t="s">
@@ -2760,8 +1827,8 @@
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="27" t="s">
+      <c r="G32" s="24"/>
+      <c r="H32" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I32" s="8" t="s">
@@ -2770,8 +1837,8 @@
       <c r="J32" s="12"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="8" t="s">
         <v>21</v>
       </c>
@@ -2780,16 +1847,16 @@
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="28"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J33" s="12"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="8" t="s">
         <v>22</v>
       </c>
@@ -2798,16 +1865,16 @@
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="29"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="30" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2818,8 +1885,8 @@
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="30" t="s">
+      <c r="G35" s="24"/>
+      <c r="H35" s="37" t="s">
         <v>6</v>
       </c>
       <c r="I35" s="10" t="s">
@@ -2828,8 +1895,8 @@
       <c r="J35" s="13"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="16" t="s">
         <v>21</v>
       </c>
@@ -2838,16 +1905,16 @@
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="31"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="10" t="s">
         <v>22</v>
       </c>
@@ -2856,18 +1923,18 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="32"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="39"/>
       <c r="I37" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -2878,10 +1945,10 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I38" s="7" t="s">
@@ -2890,8 +1957,8 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="7" t="s">
         <v>21</v>
       </c>
@@ -2900,16 +1967,16 @@
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="25"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="27"/>
       <c r="I39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="7" t="s">
         <v>22</v>
       </c>
@@ -2918,16 +1985,16 @@
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="26"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="28"/>
       <c r="I40" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="27" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -2938,8 +2005,8 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="27" t="s">
+      <c r="G41" s="24"/>
+      <c r="H41" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I41" s="8" t="s">
@@ -2948,8 +2015,8 @@
       <c r="J41" s="12"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
@@ -2958,16 +2025,16 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="28"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="35"/>
       <c r="I42" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="8" t="s">
         <v>22</v>
       </c>
@@ -2976,16 +2043,16 @@
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="29"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="36"/>
       <c r="I43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="30" t="s">
+      <c r="A44" s="24"/>
+      <c r="B44" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -2996,8 +2063,8 @@
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="30" t="s">
+      <c r="G44" s="24"/>
+      <c r="H44" s="37" t="s">
         <v>6</v>
       </c>
       <c r="I44" s="10" t="s">
@@ -3006,8 +2073,8 @@
       <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="10" t="s">
         <v>21</v>
       </c>
@@ -3016,16 +2083,16 @@
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="31"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="38"/>
       <c r="I45" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="10" t="s">
         <v>22</v>
       </c>
@@ -3034,18 +2101,18 @@
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="32"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -3056,10 +2123,10 @@
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I47" s="7" t="s">
@@ -3068,8 +2135,8 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="7" t="s">
         <v>21</v>
       </c>
@@ -3078,16 +2145,16 @@
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="25"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="27"/>
       <c r="I48" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J48" s="11"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="7" t="s">
         <v>22</v>
       </c>
@@ -3096,16 +2163,16 @@
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="26"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="28"/>
       <c r="I49" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J49" s="11"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="27" t="s">
+      <c r="A50" s="24"/>
+      <c r="B50" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="16" t="s">
@@ -3116,8 +2183,8 @@
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="27" t="s">
+      <c r="G50" s="24"/>
+      <c r="H50" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I50" s="8" t="s">
@@ -3126,8 +2193,8 @@
       <c r="J50" s="12"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="28"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="35"/>
       <c r="C51" s="8" t="s">
         <v>21</v>
       </c>
@@ -3136,16 +2203,16 @@
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="28"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="35"/>
       <c r="I51" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J51" s="12"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="8" t="s">
         <v>22</v>
       </c>
@@ -3154,16 +2221,16 @@
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="29"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="36"/>
       <c r="I52" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="12"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="30" t="s">
+      <c r="A53" s="24"/>
+      <c r="B53" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="16" t="s">
@@ -3174,8 +2241,8 @@
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="30" t="s">
+      <c r="G53" s="24"/>
+      <c r="H53" s="37" t="s">
         <v>6</v>
       </c>
       <c r="I53" s="10" t="s">
@@ -3184,8 +2251,8 @@
       <c r="J53" s="13"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="38"/>
       <c r="C54" s="10" t="s">
         <v>21</v>
       </c>
@@ -3194,16 +2261,16 @@
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="31"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="38"/>
       <c r="I54" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J54" s="13"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="32"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="39"/>
       <c r="C55" s="10" t="s">
         <v>22</v>
       </c>
@@ -3212,8 +2279,8 @@
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="32"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="39"/>
       <c r="I55" s="10" t="s">
         <v>22</v>
       </c>
@@ -3323,10 +2390,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -3335,10 +2402,10 @@
       <c r="D2" s="11">
         <v>0.57861635</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -3349,16 +2416,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="11">
         <v>0.63207546999999997</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
@@ -3367,16 +2434,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="17">
         <v>0.65094339999999995</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="26"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="16" t="s">
         <v>22</v>
       </c>
@@ -3385,8 +2452,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3395,8 +2462,8 @@
       <c r="D5" s="12">
         <v>0.69182390000000005</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="18" t="s">
@@ -3407,16 +2474,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="12">
         <v>0.66981131999999999</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="9" t="s">
         <v>21</v>
       </c>
@@ -3425,16 +2492,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="17">
         <v>0.70440252000000003</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="9" t="s">
         <v>22</v>
       </c>
@@ -3443,8 +2510,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -3453,8 +2520,8 @@
       <c r="D8" s="13">
         <v>0.73270440000000003</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="34" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="16" t="s">
@@ -3465,16 +2532,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="13">
         <v>0.66666667000000002</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="34"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="10" t="s">
         <v>21</v>
       </c>
@@ -3483,16 +2550,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="17">
         <v>0.73899371000000003</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="34"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="10" t="s">
         <v>22</v>
       </c>
@@ -3501,10 +2568,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -3515,8 +2582,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="16" t="s">
         <v>21</v>
       </c>
@@ -3525,8 +2592,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
@@ -3535,8 +2602,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -3547,8 +2614,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
@@ -3557,8 +2624,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
@@ -3567,8 +2634,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -3579,8 +2646,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="16" t="s">
         <v>21</v>
       </c>
@@ -3589,8 +2656,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
@@ -3599,10 +2666,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -3613,8 +2680,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
@@ -3623,8 +2690,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3633,8 +2700,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="27" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -3645,8 +2712,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="16" t="s">
         <v>21</v>
       </c>
@@ -3655,8 +2722,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
@@ -3665,8 +2732,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="30" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -3677,8 +2744,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="10" t="s">
         <v>21</v>
       </c>
@@ -3687,8 +2754,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
@@ -3750,10 +2817,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -3764,8 +2831,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
@@ -3774,8 +2841,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
@@ -3784,8 +2851,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3796,8 +2863,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="18" t="s">
         <v>21</v>
       </c>
@@ -3806,8 +2873,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
@@ -3816,8 +2883,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -3828,8 +2895,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
@@ -3838,8 +2905,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
@@ -3848,10 +2915,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -3862,8 +2929,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
@@ -3872,8 +2939,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
@@ -3882,8 +2949,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -3894,8 +2961,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
@@ -3904,8 +2971,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
@@ -3914,8 +2981,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -3926,8 +2993,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
@@ -3936,8 +3003,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
@@ -3946,10 +3013,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -3960,8 +3027,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
@@ -3970,8 +3037,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3980,8 +3047,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="27" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -3992,8 +3059,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="9" t="s">
         <v>21</v>
       </c>
@@ -4002,8 +3069,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
@@ -4012,8 +3079,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="30" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -4024,8 +3091,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="15" t="s">
         <v>21</v>
       </c>
@@ -4034,8 +3101,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="10" t="s">
         <v>22</v>
       </c>
@@ -4044,10 +3111,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -4058,8 +3125,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="18" t="s">
         <v>21</v>
       </c>
@@ -4068,8 +3135,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
@@ -4078,8 +3145,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="27" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -4090,8 +3157,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="9" t="s">
         <v>21</v>
       </c>
@@ -4100,8 +3167,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="16" t="s">
         <v>22</v>
       </c>
@@ -4110,8 +3177,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="30" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -4122,8 +3189,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="15" t="s">
         <v>21</v>
       </c>
@@ -4132,8 +3199,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="16" t="s">
         <v>22</v>
       </c>
@@ -4142,10 +3209,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -4156,8 +3223,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="7" t="s">
         <v>21</v>
       </c>
@@ -4166,8 +3233,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="7" t="s">
         <v>22</v>
       </c>
@@ -4176,8 +3243,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="27" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="16" t="s">
@@ -4188,8 +3255,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
@@ -4198,8 +3265,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="8" t="s">
         <v>22</v>
       </c>
@@ -4208,8 +3275,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="30" t="s">
+      <c r="A44" s="24"/>
+      <c r="B44" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="16" t="s">
@@ -4220,8 +3287,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="10" t="s">
         <v>21</v>
       </c>
@@ -4230,8 +3297,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="10" t="s">
         <v>22</v>
       </c>
@@ -4240,10 +3307,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -4254,8 +3321,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="7" t="s">
         <v>21</v>
       </c>
@@ -4264,8 +3331,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="7" t="s">
         <v>22</v>
       </c>
@@ -4274,8 +3341,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="27" t="s">
+      <c r="A50" s="24"/>
+      <c r="B50" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
@@ -4286,8 +3353,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="28"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="35"/>
       <c r="C51" s="8" t="s">
         <v>21</v>
       </c>
@@ -4296,8 +3363,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="8" t="s">
         <v>22</v>
       </c>
@@ -4306,8 +3373,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="30" t="s">
+      <c r="A53" s="24"/>
+      <c r="B53" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="10" t="s">
@@ -4318,8 +3385,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="38"/>
       <c r="C54" s="10" t="s">
         <v>21</v>
       </c>
@@ -4328,8 +3395,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="32"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="39"/>
       <c r="C55" s="10" t="s">
         <v>22</v>
       </c>

</xml_diff>